<commit_message>
price fix + incredible
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eledah\Documents\GitHub\pmonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7087E123-F84C-4704-B71B-45ECCCEAE672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A32A00-EAFE-43DF-822B-C1971A72BB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="15540" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>پنیر فتا دوشه هراز- 400 گرم</t>
   </si>
   <si>
-    <t>https://www.digikala.com/product/dkp-1485597/%D9%BE%D9%86%DB%8C%D8%B1-%D9%81%D8%AA%D8%A7-%D8%AF%D9%88%D8%B4%D9%87-%D9%87%D8%B1%D8%A7%D8%B2-%D9%85%D9%82%D8%AF%D8%A7%D8%B1-400-%DA%AF%D8%B1%D9%85/</t>
-  </si>
-  <si>
     <t>کنسرو ماهی تن در روغن مایع ساحل - 180 گرم</t>
   </si>
   <si>
@@ -237,9 +234,6 @@
     <t>سرویس 26 پارچه اپال</t>
   </si>
   <si>
-    <t>https://www.digikala.com/product/dkp-4714424/%D9%82%D8%B1%D8%B5-%D9%85%D8%A7%D8%B4%D9%8A%D9%86-%D8%B8%D8%B1%D9%81%D8%B4%D9%88%D9%8A%DB%8C-%D9%87%D9%88%D9%85-%D9%BE%D9%84%D8%A7%D8%B3-%D9%85%D8%AF%D9%84-lemon-%D8%A8%D8%B3%D8%AA%D9%87-48-%D8%B9%D8%AF%D8%AF%DB%8C/</t>
-  </si>
-  <si>
     <t>قرص ماشین ظرفشویی هوم پلاس 48 عددی</t>
   </si>
   <si>
@@ -321,12 +315,6 @@
     <t>https://www.digikala.com/product/dkp-4588938/%D9%81%DB%8C%D9%84%D9%87-%D9%85%D8%A7%D9%87%DB%8C-%D8%AD%D8%B3%D9%88%D9%86-%D8%AC%D9%86%D9%88%D8%A8-%D9%BE%D9%85%DB%8C%D9%86%D8%A7-700-%DA%AF%D8%B1%D9%85/</t>
   </si>
   <si>
-    <t>https://www.digikala.com/product/dkp-757476/%D8%B3%DB%8C%D8%A8-%D8%B2%D9%85%DB%8C%D9%86%DB%8C-%D8%B7%D9%84%D8%A7%DB%8C%DB%8C-%D9%85%D9%86%D8%AC%D9%85%D8%AF-%D8%B3%D8%B1%D8%AF-%D9%88-%D8%AA%D8%A7%D8%B2%D9%87-%D9%85%D9%82%D8%AF%D8%A7%D8%B1-750-%DA%AF%D8%B1%D9%85/</t>
-  </si>
-  <si>
-    <t>https://www.digikala.com/product/dkp-1023378/%D9%BE%D9%86%DB%8C%D8%B1-%D9%BE%DB%8C%D8%AA%D8%B2%D8%A7-%D8%AA%D8%A7%D9%BE%DB%8C%D9%86%DA%AF-%D8%A8%D8%A7-%D8%B7%D8%B9%D9%85-%D9%85%D9%88%D8%B2%D8%A7%D8%B1%D9%84%D8%A7-%D9%88-%DA%86%D8%AF%D8%A7%D8%B1-%D8%B1%D9%86%D8%AF%D9%87-%D8%B4%D8%AF%D9%87-%DA%A9%D8%A7%D9%84%DB%8C%D9%86-1000-%DA%AF%D8%B1%D9%85/</t>
-  </si>
-  <si>
     <t>پنیر پیتزا رنده شده کالین - 1000 گرم</t>
   </si>
   <si>
@@ -391,6 +379,18 @@
   </si>
   <si>
     <t>https://www.digikala.com/product/dkp-12457748/%D9%BE%D8%B3%D8%AA%D9%87-%D8%A7%DA%A9%D8%A8%D8%B1%DB%8C-%D8%AA%D8%B1%D8%AF-%D9%86%D9%85%DA%A9%DB%8C-%D8%AF%D8%B3%D8%AA-%DA%86%DB%8C%D9%86-%D8%B4%D9%88%D8%AF%DB%8C%DA%A9-1000-%DA%AF%D8%B1%D9%85/</t>
+  </si>
+  <si>
+    <t>https://www.digikala.com/fresh/product/dkp-4714424/</t>
+  </si>
+  <si>
+    <t>https://www.digikala.com/fresh/product/dkp-757476/</t>
+  </si>
+  <si>
+    <t>https://www.digikala.com/fresh/product/dkp-1023378/</t>
+  </si>
+  <si>
+    <t>https://www.digikala.com/fresh/product/dkp-1485597/</t>
   </si>
 </sst>
 </file>
@@ -711,7 +711,7 @@
   <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,18 +722,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
         <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -762,10 +762,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -778,23 +778,23 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
         <v>38</v>
@@ -810,42 +810,42 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -866,18 +866,18 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
         <v>66</v>
-      </c>
-      <c r="B19" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -890,18 +890,18 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -914,10 +914,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -930,58 +930,58 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
         <v>68</v>
-      </c>
-      <c r="B30" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -994,18 +994,18 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1018,42 +1018,42 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" t="s">
         <v>56</v>
-      </c>
-      <c r="B42" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1066,26 +1066,26 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
         <v>62</v>
-      </c>
-      <c r="B45" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1114,10 +1114,10 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1130,26 +1130,26 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
         <v>54</v>
-      </c>
-      <c r="B53" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="s">
         <v>60</v>
-      </c>
-      <c r="B54" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1162,26 +1162,26 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1194,18 +1194,18 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B61" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>